<commit_message>
update search by various attributes in Redis(cache). Revise highlighters in twitter data dictionary file (only choose hashtags in entities object and deleted quoted_status)
</commit_message>
<xml_diff>
--- a/Caching/twitter data dictionary.xlsx
+++ b/Caching/twitter data dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cyan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Dish/694final/694-2023-team18/Caching/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E343EBCC-70F5-9A42-8080-E5A0E2FAEE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002BB4E5-4CE4-3E4E-BEFA-2AC880188BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{CF9CA6ED-CC17-8A4A-9FFB-4613455172A0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{CF9CA6ED-CC17-8A4A-9FFB-4613455172A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Twitter Object" sheetId="11" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Extended entities object" sheetId="12" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1984,7 +1983,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2033,22 +2032,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2368,11 +2376,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{975B572A-4FED-8541-8AEF-02C535C15AA7}">
   <dimension ref="A1:D212"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C140" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B150" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A32" sqref="A32:A35"/>
+      <selection pane="bottomRight" activeCell="C142" sqref="C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2562,7 +2570,7 @@
       <c r="B24" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="16" t="s">
         <v>326</v>
       </c>
       <c r="D24" t="s">
@@ -2572,12 +2580,12 @@
     <row r="25" spans="1:4">
       <c r="A25" s="15"/>
       <c r="B25" s="15"/>
-      <c r="C25" s="19"/>
+      <c r="C25" s="17"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="15"/>
       <c r="B26" s="15"/>
-      <c r="C26" s="19"/>
+      <c r="C26" s="17"/>
       <c r="D26" s="8" t="s">
         <v>127</v>
       </c>
@@ -2585,7 +2593,7 @@
     <row r="27" spans="1:4" ht="59" customHeight="1">
       <c r="A27" s="15"/>
       <c r="B27" s="15"/>
-      <c r="C27" s="19"/>
+      <c r="C27" s="17"/>
       <c r="D27" s="8"/>
     </row>
     <row r="28" spans="1:4">
@@ -2727,7 +2735,7 @@
       <c r="A48" s="14" t="s">
         <v>339</v>
       </c>
-      <c r="B48" s="16" t="s">
+      <c r="B48" s="18" t="s">
         <v>11</v>
       </c>
       <c r="D48" t="s">
@@ -2736,309 +2744,309 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="14"/>
-      <c r="B49" s="16"/>
+      <c r="B49" s="18"/>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="14"/>
-      <c r="B50" s="16"/>
+      <c r="B50" s="18"/>
       <c r="D50" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="14"/>
-      <c r="B51" s="16"/>
+      <c r="B51" s="18"/>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="14"/>
-      <c r="B52" s="16"/>
+      <c r="B52" s="18"/>
       <c r="D52" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="14"/>
-      <c r="B53" s="16"/>
+      <c r="B53" s="18"/>
       <c r="D53" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="14"/>
-      <c r="B54" s="16"/>
+      <c r="B54" s="18"/>
       <c r="D54" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="14"/>
-      <c r="B55" s="16"/>
+      <c r="B55" s="18"/>
       <c r="D55" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="14"/>
-      <c r="B56" s="16"/>
+      <c r="B56" s="18"/>
       <c r="D56" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="14"/>
-      <c r="B57" s="16"/>
+      <c r="B57" s="18"/>
       <c r="D57" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="14"/>
-      <c r="B58" s="16"/>
+      <c r="B58" s="18"/>
       <c r="D58" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="14"/>
-      <c r="B59" s="16"/>
+      <c r="B59" s="18"/>
       <c r="D59" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="14"/>
-      <c r="B60" s="16"/>
+      <c r="B60" s="18"/>
       <c r="D60" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="14"/>
-      <c r="B61" s="16"/>
+      <c r="B61" s="18"/>
       <c r="D61" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="14"/>
-      <c r="B62" s="16"/>
+      <c r="B62" s="18"/>
       <c r="D62" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="14"/>
-      <c r="B63" s="16"/>
+      <c r="B63" s="18"/>
       <c r="D63" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="14"/>
-      <c r="B64" s="16"/>
+      <c r="B64" s="18"/>
       <c r="D64" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="14"/>
-      <c r="B65" s="16"/>
+      <c r="B65" s="18"/>
       <c r="D65" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="14"/>
-      <c r="B66" s="16"/>
+      <c r="B66" s="18"/>
       <c r="D66" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="14"/>
-      <c r="B67" s="16"/>
+      <c r="B67" s="18"/>
       <c r="D67" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="14"/>
-      <c r="B68" s="16"/>
+      <c r="B68" s="18"/>
       <c r="D68" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="14"/>
-      <c r="B69" s="16"/>
+      <c r="B69" s="18"/>
       <c r="D69" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="14"/>
-      <c r="B70" s="16"/>
+      <c r="B70" s="18"/>
       <c r="D70" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="14"/>
-      <c r="B71" s="16"/>
+      <c r="B71" s="18"/>
       <c r="D71" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="14"/>
-      <c r="B72" s="16"/>
+      <c r="B72" s="18"/>
       <c r="D72" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="14"/>
-      <c r="B73" s="16"/>
+      <c r="B73" s="18"/>
       <c r="D73" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="14"/>
-      <c r="B74" s="16"/>
+      <c r="B74" s="18"/>
       <c r="D74" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="14"/>
-      <c r="B75" s="16"/>
+      <c r="B75" s="18"/>
       <c r="D75" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="14"/>
-      <c r="B76" s="16"/>
+      <c r="B76" s="18"/>
       <c r="D76" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="14"/>
-      <c r="B77" s="16"/>
+      <c r="B77" s="18"/>
       <c r="D77" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="14"/>
-      <c r="B78" s="16"/>
+      <c r="B78" s="18"/>
       <c r="D78" s="8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="14"/>
-      <c r="B79" s="16"/>
+      <c r="B79" s="18"/>
       <c r="D79" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="14"/>
-      <c r="B80" s="16"/>
+      <c r="B80" s="18"/>
       <c r="D80" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="14"/>
-      <c r="B81" s="16"/>
+      <c r="B81" s="18"/>
       <c r="D81" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="14"/>
-      <c r="B82" s="16"/>
+      <c r="B82" s="18"/>
       <c r="D82" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="14"/>
-      <c r="B83" s="16"/>
+      <c r="B83" s="18"/>
       <c r="D83" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="14"/>
-      <c r="B84" s="16"/>
+      <c r="B84" s="18"/>
       <c r="D84" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="14"/>
-      <c r="B85" s="16"/>
+      <c r="B85" s="18"/>
       <c r="D85" s="8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="14"/>
-      <c r="B86" s="16"/>
+      <c r="B86" s="18"/>
       <c r="D86" s="8" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="14"/>
-      <c r="B87" s="16"/>
+      <c r="B87" s="18"/>
       <c r="D87" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="14"/>
-      <c r="B88" s="16"/>
+      <c r="B88" s="18"/>
       <c r="D88" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="14"/>
-      <c r="B89" s="16"/>
+      <c r="B89" s="18"/>
       <c r="D89" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="14"/>
-      <c r="B90" s="16"/>
+      <c r="B90" s="18"/>
       <c r="D90" s="8" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="14"/>
-      <c r="B91" s="16"/>
+      <c r="B91" s="18"/>
       <c r="D91" s="8" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="14"/>
-      <c r="B92" s="16"/>
+      <c r="B92" s="18"/>
       <c r="D92" s="8"/>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B93" s="17" t="s">
+      <c r="B93" s="19" t="s">
         <v>55</v>
       </c>
       <c r="D93" s="4" t="s">
@@ -3047,81 +3055,81 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="15"/>
-      <c r="B94" s="17"/>
+      <c r="B94" s="19"/>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="15"/>
-      <c r="B95" s="17"/>
+      <c r="B95" s="19"/>
       <c r="D95" s="8" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="15"/>
-      <c r="B96" s="17"/>
+      <c r="B96" s="19"/>
       <c r="D96" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="15"/>
-      <c r="B97" s="17"/>
+      <c r="B97" s="19"/>
       <c r="D97" s="8" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="15"/>
-      <c r="B98" s="17"/>
+      <c r="B98" s="19"/>
       <c r="D98" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="15"/>
-      <c r="B99" s="17"/>
+      <c r="B99" s="19"/>
       <c r="D99" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="15"/>
-      <c r="B100" s="17"/>
+      <c r="B100" s="19"/>
       <c r="D100" s="8">
         <v>40.057016490000002</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="15"/>
-      <c r="B101" s="17"/>
+      <c r="B101" s="19"/>
       <c r="D101" s="8" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="15"/>
-      <c r="B102" s="17"/>
+      <c r="B102" s="19"/>
       <c r="D102" s="8" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="15"/>
-      <c r="B103" s="17"/>
+      <c r="B103" s="19"/>
       <c r="D103" s="8" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="15"/>
-      <c r="B104" s="17"/>
+      <c r="B104" s="19"/>
       <c r="D104" s="8"/>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B105" s="17" t="s">
+      <c r="B105" s="19" t="s">
         <v>63</v>
       </c>
       <c r="D105" s="9" t="s">
@@ -3130,165 +3138,165 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="15"/>
-      <c r="B106" s="17"/>
+      <c r="B106" s="19"/>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="15"/>
-      <c r="B107" s="17"/>
+      <c r="B107" s="19"/>
       <c r="D107" s="8" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="15"/>
-      <c r="B108" s="17"/>
+      <c r="B108" s="19"/>
       <c r="D108" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="15"/>
-      <c r="B109" s="17"/>
+      <c r="B109" s="19"/>
       <c r="D109" s="8" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="15"/>
-      <c r="B110" s="17"/>
+      <c r="B110" s="19"/>
       <c r="D110" s="8" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="15"/>
-      <c r="B111" s="17"/>
+      <c r="B111" s="19"/>
       <c r="D111" s="8" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="15"/>
-      <c r="B112" s="17"/>
+      <c r="B112" s="19"/>
       <c r="D112" s="8" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="15"/>
-      <c r="B113" s="17"/>
+      <c r="B113" s="19"/>
       <c r="D113" s="8" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="15"/>
-      <c r="B114" s="17"/>
+      <c r="B114" s="19"/>
       <c r="D114" s="8" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="15"/>
-      <c r="B115" s="17"/>
+      <c r="B115" s="19"/>
       <c r="D115" s="8" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="15"/>
-      <c r="B116" s="17"/>
+      <c r="B116" s="19"/>
       <c r="D116" s="8" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="15"/>
-      <c r="B117" s="17"/>
+      <c r="B117" s="19"/>
       <c r="D117" s="8" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="15"/>
-      <c r="B118" s="17"/>
+      <c r="B118" s="19"/>
       <c r="D118" s="8" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="15"/>
-      <c r="B119" s="17"/>
+      <c r="B119" s="19"/>
       <c r="D119" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="15"/>
-      <c r="B120" s="17"/>
+      <c r="B120" s="19"/>
       <c r="D120" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="15"/>
-      <c r="B121" s="17"/>
+      <c r="B121" s="19"/>
       <c r="D121" s="8" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="15"/>
-      <c r="B122" s="17"/>
+      <c r="B122" s="19"/>
       <c r="D122" s="8" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="15"/>
-      <c r="B123" s="17"/>
+      <c r="B123" s="19"/>
       <c r="D123" s="8" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="15"/>
-      <c r="B124" s="17"/>
+      <c r="B124" s="19"/>
       <c r="D124" s="8" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="15"/>
-      <c r="B125" s="17"/>
+      <c r="B125" s="19"/>
       <c r="D125" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="15"/>
-      <c r="B126" s="17"/>
+      <c r="B126" s="19"/>
       <c r="D126" s="8" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="15"/>
-      <c r="B127" s="17"/>
+      <c r="B127" s="19"/>
       <c r="D127" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="15"/>
-      <c r="B128" s="17"/>
+      <c r="B128" s="19"/>
       <c r="D128" s="8" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="15"/>
-      <c r="B129" s="17"/>
+      <c r="B129" s="19"/>
       <c r="D129" s="8"/>
     </row>
     <row r="130" spans="1:4">
@@ -3373,10 +3381,10 @@
       <c r="D141" s="8"/>
     </row>
     <row r="142" spans="1:4" ht="110" customHeight="1">
-      <c r="A142" s="10" t="s">
+      <c r="A142" s="22" t="s">
         <v>341</v>
       </c>
-      <c r="B142" s="10" t="s">
+      <c r="B142" s="22" t="s">
         <v>88</v>
       </c>
       <c r="D142" t="s">
@@ -3518,7 +3526,7 @@
       <c r="A162" s="14" t="s">
         <v>347</v>
       </c>
-      <c r="B162" s="16" t="s">
+      <c r="B162" s="18" t="s">
         <v>95</v>
       </c>
       <c r="D162" s="4" t="s">
@@ -3527,81 +3535,81 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="14"/>
-      <c r="B163" s="16"/>
+      <c r="B163" s="18"/>
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="14"/>
-      <c r="B164" s="16"/>
+      <c r="B164" s="18"/>
       <c r="D164" s="8" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="14"/>
-      <c r="B165" s="16"/>
+      <c r="B165" s="18"/>
       <c r="D165" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="14"/>
-      <c r="B166" s="16"/>
+      <c r="B166" s="18"/>
       <c r="D166" s="8" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="14"/>
-      <c r="B167" s="16"/>
+      <c r="B167" s="18"/>
       <c r="D167" s="8" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="14"/>
-      <c r="B168" s="16"/>
+      <c r="B168" s="18"/>
       <c r="D168" s="8" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="14"/>
-      <c r="B169" s="16"/>
+      <c r="B169" s="18"/>
       <c r="D169" s="8" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="14"/>
-      <c r="B170" s="16"/>
+      <c r="B170" s="18"/>
       <c r="D170" s="8" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="171" spans="1:4">
       <c r="A171" s="14"/>
-      <c r="B171" s="16"/>
+      <c r="B171" s="18"/>
       <c r="D171" s="8" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="172" spans="1:4">
       <c r="A172" s="14"/>
-      <c r="B172" s="16"/>
+      <c r="B172" s="18"/>
       <c r="D172" s="8" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="173" spans="1:4">
       <c r="A173" s="14"/>
-      <c r="B173" s="16"/>
+      <c r="B173" s="18"/>
       <c r="D173" s="8"/>
     </row>
     <row r="174" spans="1:4">
       <c r="A174" s="14" t="s">
         <v>348</v>
       </c>
-      <c r="B174" s="16" t="s">
+      <c r="B174" s="18" t="s">
         <v>103</v>
       </c>
       <c r="D174" s="4" t="s">
@@ -3610,39 +3618,39 @@
     </row>
     <row r="175" spans="1:4">
       <c r="A175" s="14"/>
-      <c r="B175" s="16"/>
+      <c r="B175" s="18"/>
     </row>
     <row r="176" spans="1:4">
       <c r="A176" s="14"/>
-      <c r="B176" s="16"/>
+      <c r="B176" s="18"/>
       <c r="D176" s="8" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="177" spans="1:4">
       <c r="A177" s="14"/>
-      <c r="B177" s="16"/>
+      <c r="B177" s="18"/>
       <c r="D177" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="178" spans="1:4">
       <c r="A178" s="14"/>
-      <c r="B178" s="16"/>
+      <c r="B178" s="18"/>
       <c r="D178" s="8" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="179" spans="1:4">
       <c r="A179" s="14"/>
-      <c r="B179" s="16"/>
+      <c r="B179" s="18"/>
       <c r="D179" s="8" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="180" spans="1:4">
       <c r="A180" s="14"/>
-      <c r="B180" s="16"/>
+      <c r="B180" s="18"/>
       <c r="D180" s="8"/>
     </row>
     <row r="181" spans="1:4">
@@ -3859,6 +3867,49 @@
     </row>
   </sheetData>
   <mergeCells count="59">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="A48:A92"/>
+    <mergeCell ref="B48:B92"/>
+    <mergeCell ref="A93:A104"/>
+    <mergeCell ref="B93:B104"/>
+    <mergeCell ref="A105:A129"/>
+    <mergeCell ref="B105:B129"/>
+    <mergeCell ref="A130:A133"/>
+    <mergeCell ref="B130:B133"/>
+    <mergeCell ref="A134:A137"/>
+    <mergeCell ref="B134:B137"/>
+    <mergeCell ref="A138:A141"/>
+    <mergeCell ref="B138:B141"/>
+    <mergeCell ref="A144:A148"/>
+    <mergeCell ref="B144:B148"/>
+    <mergeCell ref="B181:B184"/>
+    <mergeCell ref="A149:A153"/>
+    <mergeCell ref="B149:B153"/>
+    <mergeCell ref="A154:A157"/>
+    <mergeCell ref="B154:B157"/>
+    <mergeCell ref="A158:A161"/>
+    <mergeCell ref="B158:B161"/>
     <mergeCell ref="A201:A204"/>
     <mergeCell ref="B201:B204"/>
     <mergeCell ref="A205:A212"/>
@@ -3875,49 +3926,6 @@
     <mergeCell ref="A174:A180"/>
     <mergeCell ref="B174:B180"/>
     <mergeCell ref="A181:A184"/>
-    <mergeCell ref="B181:B184"/>
-    <mergeCell ref="A149:A153"/>
-    <mergeCell ref="B149:B153"/>
-    <mergeCell ref="A154:A157"/>
-    <mergeCell ref="B154:B157"/>
-    <mergeCell ref="A158:A161"/>
-    <mergeCell ref="B158:B161"/>
-    <mergeCell ref="A134:A137"/>
-    <mergeCell ref="B134:B137"/>
-    <mergeCell ref="A138:A141"/>
-    <mergeCell ref="B138:B141"/>
-    <mergeCell ref="A144:A148"/>
-    <mergeCell ref="B144:B148"/>
-    <mergeCell ref="A93:A104"/>
-    <mergeCell ref="B93:B104"/>
-    <mergeCell ref="A105:A129"/>
-    <mergeCell ref="B105:B129"/>
-    <mergeCell ref="A130:A133"/>
-    <mergeCell ref="B130:B133"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="A48:A92"/>
-    <mergeCell ref="B48:B92"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -4485,6 +4493,42 @@
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B38:B40"/>
     <mergeCell ref="A51:A54"/>
     <mergeCell ref="B51:B54"/>
     <mergeCell ref="A41:A42"/>
@@ -4493,42 +4537,6 @@
     <mergeCell ref="B43:B44"/>
     <mergeCell ref="A45:A50"/>
     <mergeCell ref="B45:B50"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -4547,11 +4555,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEAF76D1-ED53-D146-BC1A-7722F4D40657}">
   <dimension ref="A1:C139"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A106" sqref="A106:B117"/>
+      <selection pane="bottomRight" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4577,7 +4585,7 @@
       <c r="A2" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="18" t="s">
         <v>299</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -4586,86 +4594,86 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="21"/>
-      <c r="B3" s="16"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="21"/>
-      <c r="B4" s="16"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="3" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="21"/>
-      <c r="B5" s="16"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="3" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="21"/>
-      <c r="B6" s="16"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="3" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="21"/>
-      <c r="B7" s="16"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="3" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="21"/>
-      <c r="B8" s="16"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="3">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="21"/>
-      <c r="B9" s="16"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="3" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="21"/>
-      <c r="B10" s="16"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="3" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="21"/>
-      <c r="B11" s="16"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="3" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="21"/>
-      <c r="B12" s="16"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="3" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="21"/>
-      <c r="B13" s="16"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="23" t="s">
         <v>216</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="24" t="s">
         <v>300</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -4673,290 +4681,290 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="21"/>
-      <c r="B15" s="16"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="21"/>
-      <c r="B16" s="16"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="24"/>
       <c r="C16" s="3" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="21"/>
-      <c r="B17" s="16"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="24"/>
       <c r="C17" s="3" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="21"/>
-      <c r="B18" s="16"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="24"/>
       <c r="C18" s="3" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="21"/>
-      <c r="B19" s="16"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="3" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="21"/>
-      <c r="B20" s="16"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="24"/>
       <c r="C20" s="3" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="21"/>
-      <c r="B21" s="16"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="24"/>
       <c r="C21" s="3" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="21"/>
-      <c r="B22" s="16"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="3" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="21"/>
-      <c r="B23" s="16"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="24"/>
       <c r="C23" s="3" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="21"/>
-      <c r="B24" s="16"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="24"/>
       <c r="C24" s="3">
         <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="21"/>
-      <c r="B25" s="16"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="24"/>
       <c r="C25" s="3" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="21"/>
-      <c r="B26" s="16"/>
+      <c r="A26" s="23"/>
+      <c r="B26" s="24"/>
       <c r="C26" s="3" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="21"/>
-      <c r="B27" s="16"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="24"/>
       <c r="C27" s="3" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="21"/>
-      <c r="B28" s="16"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="24"/>
       <c r="C28" s="3" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="21"/>
-      <c r="B29" s="16"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="24"/>
       <c r="C29" s="3" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="21"/>
-      <c r="B30" s="16"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="24"/>
       <c r="C30" s="3" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="21"/>
-      <c r="B31" s="16"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="24"/>
       <c r="C31" s="3" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="21"/>
-      <c r="B32" s="16"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="24"/>
       <c r="C32" s="3" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="21"/>
-      <c r="B33" s="16"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="24"/>
       <c r="C33" s="3" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="21"/>
-      <c r="B34" s="16"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="24"/>
       <c r="C34" s="3" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="21"/>
-      <c r="B35" s="16"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="24"/>
       <c r="C35" s="3" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="21"/>
-      <c r="B36" s="16"/>
+      <c r="A36" s="23"/>
+      <c r="B36" s="24"/>
       <c r="C36" s="3" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="21"/>
-      <c r="B37" s="16"/>
+      <c r="A37" s="23"/>
+      <c r="B37" s="24"/>
       <c r="C37" s="3" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="21"/>
-      <c r="B38" s="16"/>
+      <c r="A38" s="23"/>
+      <c r="B38" s="24"/>
       <c r="C38" s="3" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="21"/>
-      <c r="B39" s="16"/>
+      <c r="A39" s="23"/>
+      <c r="B39" s="24"/>
       <c r="C39" s="3" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="21"/>
-      <c r="B40" s="16"/>
+      <c r="A40" s="23"/>
+      <c r="B40" s="24"/>
       <c r="C40" s="3" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="21"/>
-      <c r="B41" s="16"/>
+      <c r="A41" s="23"/>
+      <c r="B41" s="24"/>
       <c r="C41" s="3" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="21"/>
-      <c r="B42" s="16"/>
+      <c r="A42" s="23"/>
+      <c r="B42" s="24"/>
       <c r="C42" s="3" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="21"/>
-      <c r="B43" s="16"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="24"/>
       <c r="C43" s="3" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="21"/>
-      <c r="B44" s="16"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="24"/>
       <c r="C44" s="3" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="21"/>
-      <c r="B45" s="16"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="24"/>
       <c r="C45" s="3" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="21"/>
-      <c r="B46" s="16"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="24"/>
       <c r="C46" s="3" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="21"/>
-      <c r="B47" s="16"/>
+      <c r="A47" s="23"/>
+      <c r="B47" s="24"/>
       <c r="C47" s="3" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="21"/>
-      <c r="B48" s="16"/>
+      <c r="A48" s="23"/>
+      <c r="B48" s="24"/>
       <c r="C48" s="3" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="21"/>
-      <c r="B49" s="16"/>
+      <c r="A49" s="23"/>
+      <c r="B49" s="24"/>
       <c r="C49" s="3" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="21"/>
-      <c r="B50" s="16"/>
+      <c r="A50" s="23"/>
+      <c r="B50" s="24"/>
       <c r="C50" s="3" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="21"/>
-      <c r="B51" s="16"/>
+      <c r="A51" s="23"/>
+      <c r="B51" s="24"/>
       <c r="C51" s="3" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="21"/>
-      <c r="B52" s="16"/>
+      <c r="A52" s="23"/>
+      <c r="B52" s="24"/>
       <c r="C52" s="3" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="21"/>
-      <c r="B53" s="16"/>
+      <c r="A53" s="23"/>
+      <c r="B53" s="24"/>
       <c r="C53" s="3" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="21"/>
-      <c r="B54" s="16"/>
+      <c r="A54" s="23"/>
+      <c r="B54" s="24"/>
       <c r="C54" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="18">
-      <c r="A55" s="21" t="s">
+      <c r="A55" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="B55" s="16" t="s">
+      <c r="B55" s="24" t="s">
         <v>301</v>
       </c>
       <c r="C55" s="2" t="s">
@@ -4964,249 +4972,249 @@
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="21"/>
-      <c r="B56" s="16"/>
+      <c r="A56" s="23"/>
+      <c r="B56" s="24"/>
     </row>
     <row r="57" spans="1:3" ht="18">
-      <c r="A57" s="21"/>
-      <c r="B57" s="16"/>
+      <c r="A57" s="23"/>
+      <c r="B57" s="24"/>
       <c r="C57" s="2" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="21"/>
-      <c r="B58" s="16"/>
+      <c r="A58" s="23"/>
+      <c r="B58" s="24"/>
       <c r="C58" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="21"/>
-      <c r="B59" s="16"/>
+      <c r="A59" s="23"/>
+      <c r="B59" s="24"/>
       <c r="C59" s="3" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="21"/>
-      <c r="B60" s="16"/>
+      <c r="A60" s="23"/>
+      <c r="B60" s="24"/>
       <c r="C60" s="3" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="21"/>
-      <c r="B61" s="16"/>
+      <c r="A61" s="23"/>
+      <c r="B61" s="24"/>
       <c r="C61" s="3" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="21"/>
-      <c r="B62" s="16"/>
+      <c r="A62" s="23"/>
+      <c r="B62" s="24"/>
       <c r="C62" s="3" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="21"/>
-      <c r="B63" s="16"/>
+      <c r="A63" s="23"/>
+      <c r="B63" s="24"/>
       <c r="C63" s="3">
         <v>52</v>
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="21"/>
-      <c r="B64" s="16"/>
+      <c r="A64" s="23"/>
+      <c r="B64" s="24"/>
       <c r="C64" s="3" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="21"/>
-      <c r="B65" s="16"/>
+      <c r="A65" s="23"/>
+      <c r="B65" s="24"/>
       <c r="C65" s="3" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="21"/>
-      <c r="B66" s="16"/>
+      <c r="A66" s="23"/>
+      <c r="B66" s="24"/>
       <c r="C66" s="3" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="21"/>
-      <c r="B67" s="16"/>
+      <c r="A67" s="23"/>
+      <c r="B67" s="24"/>
       <c r="C67" s="3" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="21"/>
-      <c r="B68" s="16"/>
+      <c r="A68" s="23"/>
+      <c r="B68" s="24"/>
       <c r="C68" s="3" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="21"/>
-      <c r="B69" s="16"/>
+      <c r="A69" s="23"/>
+      <c r="B69" s="24"/>
       <c r="C69" s="3" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="21"/>
-      <c r="B70" s="16"/>
+      <c r="A70" s="23"/>
+      <c r="B70" s="24"/>
       <c r="C70" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="21"/>
-      <c r="B71" s="16"/>
+      <c r="A71" s="23"/>
+      <c r="B71" s="24"/>
     </row>
     <row r="72" spans="1:3" ht="18">
-      <c r="A72" s="21"/>
-      <c r="B72" s="16"/>
+      <c r="A72" s="23"/>
+      <c r="B72" s="24"/>
       <c r="C72" s="2" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="21"/>
-      <c r="B73" s="16"/>
+      <c r="A73" s="23"/>
+      <c r="B73" s="24"/>
       <c r="C73" s="3" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="21"/>
-      <c r="B74" s="16"/>
+      <c r="A74" s="23"/>
+      <c r="B74" s="24"/>
       <c r="C74" s="3" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="21"/>
-      <c r="B75" s="16"/>
+      <c r="A75" s="23"/>
+      <c r="B75" s="24"/>
       <c r="C75" s="3" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="21"/>
-      <c r="B76" s="16"/>
+      <c r="A76" s="23"/>
+      <c r="B76" s="24"/>
       <c r="C76" s="3" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="21"/>
-      <c r="B77" s="16"/>
+      <c r="A77" s="23"/>
+      <c r="B77" s="24"/>
       <c r="C77" s="3" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="21"/>
-      <c r="B78" s="16"/>
+      <c r="A78" s="23"/>
+      <c r="B78" s="24"/>
       <c r="C78" s="3" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" s="21"/>
-      <c r="B79" s="16"/>
+      <c r="A79" s="23"/>
+      <c r="B79" s="24"/>
       <c r="C79" s="3" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" s="21"/>
-      <c r="B80" s="16"/>
+      <c r="A80" s="23"/>
+      <c r="B80" s="24"/>
       <c r="C80" s="3" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" s="21"/>
-      <c r="B81" s="16"/>
+      <c r="A81" s="23"/>
+      <c r="B81" s="24"/>
       <c r="C81" s="3" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="21"/>
-      <c r="B82" s="16"/>
+      <c r="A82" s="23"/>
+      <c r="B82" s="24"/>
       <c r="C82" s="3" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="21"/>
-      <c r="B83" s="16"/>
+      <c r="A83" s="23"/>
+      <c r="B83" s="24"/>
       <c r="C83" s="3" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" s="21"/>
-      <c r="B84" s="16"/>
+      <c r="A84" s="23"/>
+      <c r="B84" s="24"/>
       <c r="C84" s="3" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="21"/>
-      <c r="B85" s="16"/>
+      <c r="A85" s="23"/>
+      <c r="B85" s="24"/>
       <c r="C85" s="3" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="21"/>
-      <c r="B86" s="16"/>
+      <c r="A86" s="23"/>
+      <c r="B86" s="24"/>
       <c r="C86" s="3">
         <v>85</v>
       </c>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="21"/>
-      <c r="B87" s="16"/>
+      <c r="A87" s="23"/>
+      <c r="B87" s="24"/>
       <c r="C87" s="3" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" s="21"/>
-      <c r="B88" s="16"/>
+      <c r="A88" s="23"/>
+      <c r="B88" s="24"/>
       <c r="C88" s="3" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="21"/>
-      <c r="B89" s="16"/>
+      <c r="A89" s="23"/>
+      <c r="B89" s="24"/>
       <c r="C89" s="3" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" s="21"/>
-      <c r="B90" s="16"/>
+      <c r="A90" s="23"/>
+      <c r="B90" s="24"/>
       <c r="C90" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="18">
-      <c r="A91" s="21" t="s">
+      <c r="A91" s="23" t="s">
         <v>270</v>
       </c>
-      <c r="B91" s="16" t="s">
+      <c r="B91" s="24" t="s">
         <v>302</v>
       </c>
       <c r="C91" s="2" t="s">
@@ -5214,108 +5222,108 @@
       </c>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92" s="21"/>
-      <c r="B92" s="16"/>
+      <c r="A92" s="23"/>
+      <c r="B92" s="24"/>
       <c r="C92" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" s="21"/>
-      <c r="B93" s="16"/>
+      <c r="A93" s="23"/>
+      <c r="B93" s="24"/>
       <c r="C93" s="3" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" s="21"/>
-      <c r="B94" s="16"/>
+      <c r="A94" s="23"/>
+      <c r="B94" s="24"/>
       <c r="C94" s="3" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" s="21"/>
-      <c r="B95" s="16"/>
+      <c r="A95" s="23"/>
+      <c r="B95" s="24"/>
       <c r="C95" s="3" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" s="21"/>
-      <c r="B96" s="16"/>
+      <c r="A96" s="23"/>
+      <c r="B96" s="24"/>
       <c r="C96" s="3" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="21"/>
-      <c r="B97" s="16"/>
+      <c r="A97" s="23"/>
+      <c r="B97" s="24"/>
       <c r="C97" s="3" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" s="21"/>
-      <c r="B98" s="16"/>
+      <c r="A98" s="23"/>
+      <c r="B98" s="24"/>
       <c r="C98" s="3">
         <v>15</v>
       </c>
     </row>
     <row r="99" spans="1:3">
-      <c r="A99" s="21"/>
-      <c r="B99" s="16"/>
+      <c r="A99" s="23"/>
+      <c r="B99" s="24"/>
       <c r="C99" s="3" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="100" spans="1:3">
-      <c r="A100" s="21"/>
-      <c r="B100" s="16"/>
+      <c r="A100" s="23"/>
+      <c r="B100" s="24"/>
       <c r="C100" s="3" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="101" spans="1:3">
-      <c r="A101" s="21"/>
-      <c r="B101" s="16"/>
+      <c r="A101" s="23"/>
+      <c r="B101" s="24"/>
       <c r="C101" s="3" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="102" spans="1:3">
-      <c r="A102" s="21"/>
-      <c r="B102" s="16"/>
+      <c r="A102" s="23"/>
+      <c r="B102" s="24"/>
       <c r="C102" s="3" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="103" spans="1:3">
-      <c r="A103" s="21"/>
-      <c r="B103" s="16"/>
+      <c r="A103" s="23"/>
+      <c r="B103" s="24"/>
       <c r="C103" s="3" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="104" spans="1:3">
-      <c r="A104" s="21"/>
-      <c r="B104" s="16"/>
+      <c r="A104" s="23"/>
+      <c r="B104" s="24"/>
       <c r="C104" s="3" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="105" spans="1:3">
-      <c r="A105" s="21"/>
-      <c r="B105" s="16"/>
+      <c r="A105" s="23"/>
+      <c r="B105" s="24"/>
       <c r="C105" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="18">
-      <c r="A106" s="21" t="s">
+      <c r="A106" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="B106" s="16" t="s">
+      <c r="B106" s="24" t="s">
         <v>303</v>
       </c>
       <c r="C106" s="2" t="s">
@@ -5323,87 +5331,87 @@
       </c>
     </row>
     <row r="107" spans="1:3">
-      <c r="A107" s="21"/>
-      <c r="B107" s="16"/>
+      <c r="A107" s="23"/>
+      <c r="B107" s="24"/>
       <c r="C107" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="108" spans="1:3">
-      <c r="A108" s="21"/>
-      <c r="B108" s="16"/>
+      <c r="A108" s="23"/>
+      <c r="B108" s="24"/>
       <c r="C108" s="3" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="109" spans="1:3">
-      <c r="A109" s="21"/>
-      <c r="B109" s="16"/>
+      <c r="A109" s="23"/>
+      <c r="B109" s="24"/>
       <c r="C109" s="3" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="110" spans="1:3">
-      <c r="A110" s="21"/>
-      <c r="B110" s="16"/>
+      <c r="A110" s="23"/>
+      <c r="B110" s="24"/>
       <c r="C110" s="3" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="111" spans="1:3">
-      <c r="A111" s="21"/>
-      <c r="B111" s="16"/>
+      <c r="A111" s="23"/>
+      <c r="B111" s="24"/>
       <c r="C111" s="3" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="112" spans="1:3">
-      <c r="A112" s="21"/>
-      <c r="B112" s="16"/>
+      <c r="A112" s="23"/>
+      <c r="B112" s="24"/>
       <c r="C112" s="3">
         <v>17</v>
       </c>
     </row>
     <row r="113" spans="1:3">
-      <c r="A113" s="21"/>
-      <c r="B113" s="16"/>
+      <c r="A113" s="23"/>
+      <c r="B113" s="24"/>
       <c r="C113" s="3" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="114" spans="1:3">
-      <c r="A114" s="21"/>
-      <c r="B114" s="16"/>
+      <c r="A114" s="23"/>
+      <c r="B114" s="24"/>
       <c r="C114" s="3" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="115" spans="1:3">
-      <c r="A115" s="21"/>
-      <c r="B115" s="16"/>
+      <c r="A115" s="23"/>
+      <c r="B115" s="24"/>
       <c r="C115" s="3" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="116" spans="1:3">
-      <c r="A116" s="21"/>
-      <c r="B116" s="16"/>
+      <c r="A116" s="23"/>
+      <c r="B116" s="24"/>
       <c r="C116" s="3" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="117" spans="1:3">
-      <c r="A117" s="21"/>
-      <c r="B117" s="16"/>
+      <c r="A117" s="23"/>
+      <c r="B117" s="24"/>
       <c r="C117" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="18">
-      <c r="A118" s="21" t="s">
+      <c r="A118" s="23" t="s">
         <v>283</v>
       </c>
-      <c r="B118" s="16" t="s">
+      <c r="B118" s="24" t="s">
         <v>304</v>
       </c>
       <c r="C118" s="2" t="s">
@@ -5411,166 +5419,166 @@
       </c>
     </row>
     <row r="119" spans="1:3">
-      <c r="A119" s="21"/>
-      <c r="B119" s="16"/>
+      <c r="A119" s="23"/>
+      <c r="B119" s="24"/>
       <c r="C119" s="3" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="120" spans="1:3">
-      <c r="A120" s="21"/>
-      <c r="B120" s="16"/>
+      <c r="A120" s="23"/>
+      <c r="B120" s="24"/>
       <c r="C120" s="3" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="121" spans="1:3">
-      <c r="A121" s="21"/>
-      <c r="B121" s="16"/>
+      <c r="A121" s="23"/>
+      <c r="B121" s="24"/>
       <c r="C121" s="3" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="122" spans="1:3">
-      <c r="A122" s="21"/>
-      <c r="B122" s="16"/>
+      <c r="A122" s="23"/>
+      <c r="B122" s="24"/>
       <c r="C122" s="3" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="123" spans="1:3">
-      <c r="A123" s="21"/>
-      <c r="B123" s="16"/>
+      <c r="A123" s="23"/>
+      <c r="B123" s="24"/>
       <c r="C123" s="3" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="124" spans="1:3">
-      <c r="A124" s="21"/>
-      <c r="B124" s="16"/>
+      <c r="A124" s="23"/>
+      <c r="B124" s="24"/>
       <c r="C124" s="3" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="125" spans="1:3">
-      <c r="A125" s="21"/>
-      <c r="B125" s="16"/>
+      <c r="A125" s="23"/>
+      <c r="B125" s="24"/>
       <c r="C125" s="3" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="126" spans="1:3">
-      <c r="A126" s="21"/>
-      <c r="B126" s="16"/>
+      <c r="A126" s="23"/>
+      <c r="B126" s="24"/>
       <c r="C126" s="3" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="127" spans="1:3">
-      <c r="A127" s="21"/>
-      <c r="B127" s="16"/>
+      <c r="A127" s="23"/>
+      <c r="B127" s="24"/>
       <c r="C127" s="3" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="128" spans="1:3">
-      <c r="A128" s="21"/>
-      <c r="B128" s="16"/>
+      <c r="A128" s="23"/>
+      <c r="B128" s="24"/>
       <c r="C128" s="3" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="129" spans="1:3">
-      <c r="A129" s="21"/>
-      <c r="B129" s="16"/>
+      <c r="A129" s="23"/>
+      <c r="B129" s="24"/>
       <c r="C129" s="3" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="130" spans="1:3">
-      <c r="A130" s="21"/>
-      <c r="B130" s="16"/>
+      <c r="A130" s="23"/>
+      <c r="B130" s="24"/>
       <c r="C130" s="3" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="131" spans="1:3">
-      <c r="A131" s="21"/>
-      <c r="B131" s="16"/>
+      <c r="A131" s="23"/>
+      <c r="B131" s="24"/>
       <c r="C131" s="3" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="132" spans="1:3">
-      <c r="A132" s="21"/>
-      <c r="B132" s="16"/>
+      <c r="A132" s="23"/>
+      <c r="B132" s="24"/>
       <c r="C132" s="3" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="133" spans="1:3">
-      <c r="A133" s="21"/>
-      <c r="B133" s="16"/>
+      <c r="A133" s="23"/>
+      <c r="B133" s="24"/>
       <c r="C133" s="3" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="134" spans="1:3">
-      <c r="A134" s="21"/>
-      <c r="B134" s="16"/>
+      <c r="A134" s="23"/>
+      <c r="B134" s="24"/>
       <c r="C134" s="3" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="135" spans="1:3">
-      <c r="A135" s="21"/>
-      <c r="B135" s="16"/>
+      <c r="A135" s="23"/>
+      <c r="B135" s="24"/>
       <c r="C135" s="3" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="136" spans="1:3">
-      <c r="A136" s="21"/>
-      <c r="B136" s="16"/>
+      <c r="A136" s="23"/>
+      <c r="B136" s="24"/>
       <c r="C136" s="3" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="137" spans="1:3">
-      <c r="A137" s="21"/>
-      <c r="B137" s="16"/>
+      <c r="A137" s="23"/>
+      <c r="B137" s="24"/>
       <c r="C137" s="3" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="138" spans="1:3">
-      <c r="A138" s="21"/>
-      <c r="B138" s="16"/>
+      <c r="A138" s="23"/>
+      <c r="B138" s="24"/>
       <c r="C138" s="3" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="139" spans="1:3">
-      <c r="A139" s="21"/>
-      <c r="B139" s="16"/>
+      <c r="A139" s="23"/>
+      <c r="B139" s="24"/>
       <c r="C139" s="3" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A54"/>
+    <mergeCell ref="B14:B54"/>
+    <mergeCell ref="A55:A90"/>
+    <mergeCell ref="B55:B90"/>
     <mergeCell ref="A91:A105"/>
     <mergeCell ref="B91:B105"/>
     <mergeCell ref="A106:A117"/>
     <mergeCell ref="B106:B117"/>
     <mergeCell ref="A118:A139"/>
     <mergeCell ref="B118:B139"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A54"/>
-    <mergeCell ref="B14:B54"/>
-    <mergeCell ref="A55:A90"/>
-    <mergeCell ref="B55:B90"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
python dictionary as cache
</commit_message>
<xml_diff>
--- a/Caching/twitter data dictionary.xlsx
+++ b/Caching/twitter data dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Dish/694final/694-2023-team18/Caching/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002BB4E5-4CE4-3E4E-BEFA-2AC880188BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3161553-7ADA-3345-805F-EDDD19954B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{CF9CA6ED-CC17-8A4A-9FFB-4613455172A0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{CF9CA6ED-CC17-8A4A-9FFB-4613455172A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Twitter Object" sheetId="11" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="361">
   <si>
     <t>String</t>
   </si>
@@ -1844,6 +1844,10 @@
   </si>
   <si>
     <t>statuses_count</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1983,7 +1987,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2032,28 +2036,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1">
@@ -2570,7 +2568,7 @@
       <c r="B24" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="18" t="s">
         <v>326</v>
       </c>
       <c r="D24" t="s">
@@ -2580,12 +2578,12 @@
     <row r="25" spans="1:4">
       <c r="A25" s="15"/>
       <c r="B25" s="15"/>
-      <c r="C25" s="17"/>
+      <c r="C25" s="19"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="15"/>
       <c r="B26" s="15"/>
-      <c r="C26" s="17"/>
+      <c r="C26" s="19"/>
       <c r="D26" s="8" t="s">
         <v>127</v>
       </c>
@@ -2593,7 +2591,7 @@
     <row r="27" spans="1:4" ht="59" customHeight="1">
       <c r="A27" s="15"/>
       <c r="B27" s="15"/>
-      <c r="C27" s="17"/>
+      <c r="C27" s="19"/>
       <c r="D27" s="8"/>
     </row>
     <row r="28" spans="1:4">
@@ -2735,7 +2733,7 @@
       <c r="A48" s="14" t="s">
         <v>339</v>
       </c>
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="16" t="s">
         <v>11</v>
       </c>
       <c r="D48" t="s">
@@ -2744,309 +2742,309 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="14"/>
-      <c r="B49" s="18"/>
+      <c r="B49" s="16"/>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="14"/>
-      <c r="B50" s="18"/>
+      <c r="B50" s="16"/>
       <c r="D50" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="14"/>
-      <c r="B51" s="18"/>
+      <c r="B51" s="16"/>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="14"/>
-      <c r="B52" s="18"/>
+      <c r="B52" s="16"/>
       <c r="D52" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="14"/>
-      <c r="B53" s="18"/>
+      <c r="B53" s="16"/>
       <c r="D53" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="14"/>
-      <c r="B54" s="18"/>
+      <c r="B54" s="16"/>
       <c r="D54" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="14"/>
-      <c r="B55" s="18"/>
+      <c r="B55" s="16"/>
       <c r="D55" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="14"/>
-      <c r="B56" s="18"/>
+      <c r="B56" s="16"/>
       <c r="D56" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="14"/>
-      <c r="B57" s="18"/>
+      <c r="B57" s="16"/>
       <c r="D57" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="14"/>
-      <c r="B58" s="18"/>
+      <c r="B58" s="16"/>
       <c r="D58" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="14"/>
-      <c r="B59" s="18"/>
+      <c r="B59" s="16"/>
       <c r="D59" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="14"/>
-      <c r="B60" s="18"/>
+      <c r="B60" s="16"/>
       <c r="D60" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="14"/>
-      <c r="B61" s="18"/>
+      <c r="B61" s="16"/>
       <c r="D61" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="14"/>
-      <c r="B62" s="18"/>
+      <c r="B62" s="16"/>
       <c r="D62" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="14"/>
-      <c r="B63" s="18"/>
+      <c r="B63" s="16"/>
       <c r="D63" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="14"/>
-      <c r="B64" s="18"/>
+      <c r="B64" s="16"/>
       <c r="D64" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="14"/>
-      <c r="B65" s="18"/>
+      <c r="B65" s="16"/>
       <c r="D65" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="14"/>
-      <c r="B66" s="18"/>
+      <c r="B66" s="16"/>
       <c r="D66" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="14"/>
-      <c r="B67" s="18"/>
+      <c r="B67" s="16"/>
       <c r="D67" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="14"/>
-      <c r="B68" s="18"/>
+      <c r="B68" s="16"/>
       <c r="D68" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="14"/>
-      <c r="B69" s="18"/>
+      <c r="B69" s="16"/>
       <c r="D69" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="14"/>
-      <c r="B70" s="18"/>
+      <c r="B70" s="16"/>
       <c r="D70" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="14"/>
-      <c r="B71" s="18"/>
+      <c r="B71" s="16"/>
       <c r="D71" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="14"/>
-      <c r="B72" s="18"/>
+      <c r="B72" s="16"/>
       <c r="D72" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="14"/>
-      <c r="B73" s="18"/>
+      <c r="B73" s="16"/>
       <c r="D73" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="14"/>
-      <c r="B74" s="18"/>
+      <c r="B74" s="16"/>
       <c r="D74" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="14"/>
-      <c r="B75" s="18"/>
+      <c r="B75" s="16"/>
       <c r="D75" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="14"/>
-      <c r="B76" s="18"/>
+      <c r="B76" s="16"/>
       <c r="D76" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="14"/>
-      <c r="B77" s="18"/>
+      <c r="B77" s="16"/>
       <c r="D77" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="14"/>
-      <c r="B78" s="18"/>
+      <c r="B78" s="16"/>
       <c r="D78" s="8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="14"/>
-      <c r="B79" s="18"/>
+      <c r="B79" s="16"/>
       <c r="D79" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="14"/>
-      <c r="B80" s="18"/>
+      <c r="B80" s="16"/>
       <c r="D80" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="14"/>
-      <c r="B81" s="18"/>
+      <c r="B81" s="16"/>
       <c r="D81" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="14"/>
-      <c r="B82" s="18"/>
+      <c r="B82" s="16"/>
       <c r="D82" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="14"/>
-      <c r="B83" s="18"/>
+      <c r="B83" s="16"/>
       <c r="D83" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="14"/>
-      <c r="B84" s="18"/>
+      <c r="B84" s="16"/>
       <c r="D84" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="14"/>
-      <c r="B85" s="18"/>
+      <c r="B85" s="16"/>
       <c r="D85" s="8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="14"/>
-      <c r="B86" s="18"/>
+      <c r="B86" s="16"/>
       <c r="D86" s="8" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="14"/>
-      <c r="B87" s="18"/>
+      <c r="B87" s="16"/>
       <c r="D87" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="14"/>
-      <c r="B88" s="18"/>
+      <c r="B88" s="16"/>
       <c r="D88" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="14"/>
-      <c r="B89" s="18"/>
+      <c r="B89" s="16"/>
       <c r="D89" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="14"/>
-      <c r="B90" s="18"/>
+      <c r="B90" s="16"/>
       <c r="D90" s="8" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="14"/>
-      <c r="B91" s="18"/>
+      <c r="B91" s="16"/>
       <c r="D91" s="8" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="14"/>
-      <c r="B92" s="18"/>
+      <c r="B92" s="16"/>
       <c r="D92" s="8"/>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B93" s="19" t="s">
+      <c r="B93" s="17" t="s">
         <v>55</v>
       </c>
       <c r="D93" s="4" t="s">
@@ -3055,81 +3053,81 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="15"/>
-      <c r="B94" s="19"/>
+      <c r="B94" s="17"/>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="15"/>
-      <c r="B95" s="19"/>
+      <c r="B95" s="17"/>
       <c r="D95" s="8" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="15"/>
-      <c r="B96" s="19"/>
+      <c r="B96" s="17"/>
       <c r="D96" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="15"/>
-      <c r="B97" s="19"/>
+      <c r="B97" s="17"/>
       <c r="D97" s="8" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="15"/>
-      <c r="B98" s="19"/>
+      <c r="B98" s="17"/>
       <c r="D98" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="15"/>
-      <c r="B99" s="19"/>
+      <c r="B99" s="17"/>
       <c r="D99" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="15"/>
-      <c r="B100" s="19"/>
+      <c r="B100" s="17"/>
       <c r="D100" s="8">
         <v>40.057016490000002</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="15"/>
-      <c r="B101" s="19"/>
+      <c r="B101" s="17"/>
       <c r="D101" s="8" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="15"/>
-      <c r="B102" s="19"/>
+      <c r="B102" s="17"/>
       <c r="D102" s="8" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="15"/>
-      <c r="B103" s="19"/>
+      <c r="B103" s="17"/>
       <c r="D103" s="8" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="15"/>
-      <c r="B104" s="19"/>
+      <c r="B104" s="17"/>
       <c r="D104" s="8"/>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B105" s="19" t="s">
+      <c r="B105" s="17" t="s">
         <v>63</v>
       </c>
       <c r="D105" s="9" t="s">
@@ -3138,165 +3136,165 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="15"/>
-      <c r="B106" s="19"/>
+      <c r="B106" s="17"/>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="15"/>
-      <c r="B107" s="19"/>
+      <c r="B107" s="17"/>
       <c r="D107" s="8" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="15"/>
-      <c r="B108" s="19"/>
+      <c r="B108" s="17"/>
       <c r="D108" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="15"/>
-      <c r="B109" s="19"/>
+      <c r="B109" s="17"/>
       <c r="D109" s="8" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="15"/>
-      <c r="B110" s="19"/>
+      <c r="B110" s="17"/>
       <c r="D110" s="8" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="15"/>
-      <c r="B111" s="19"/>
+      <c r="B111" s="17"/>
       <c r="D111" s="8" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="15"/>
-      <c r="B112" s="19"/>
+      <c r="B112" s="17"/>
       <c r="D112" s="8" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="15"/>
-      <c r="B113" s="19"/>
+      <c r="B113" s="17"/>
       <c r="D113" s="8" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="15"/>
-      <c r="B114" s="19"/>
+      <c r="B114" s="17"/>
       <c r="D114" s="8" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="15"/>
-      <c r="B115" s="19"/>
+      <c r="B115" s="17"/>
       <c r="D115" s="8" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="15"/>
-      <c r="B116" s="19"/>
+      <c r="B116" s="17"/>
       <c r="D116" s="8" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="15"/>
-      <c r="B117" s="19"/>
+      <c r="B117" s="17"/>
       <c r="D117" s="8" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="15"/>
-      <c r="B118" s="19"/>
+      <c r="B118" s="17"/>
       <c r="D118" s="8" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="15"/>
-      <c r="B119" s="19"/>
+      <c r="B119" s="17"/>
       <c r="D119" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="15"/>
-      <c r="B120" s="19"/>
+      <c r="B120" s="17"/>
       <c r="D120" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="15"/>
-      <c r="B121" s="19"/>
+      <c r="B121" s="17"/>
       <c r="D121" s="8" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="15"/>
-      <c r="B122" s="19"/>
+      <c r="B122" s="17"/>
       <c r="D122" s="8" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="15"/>
-      <c r="B123" s="19"/>
+      <c r="B123" s="17"/>
       <c r="D123" s="8" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="15"/>
-      <c r="B124" s="19"/>
+      <c r="B124" s="17"/>
       <c r="D124" s="8" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="15"/>
-      <c r="B125" s="19"/>
+      <c r="B125" s="17"/>
       <c r="D125" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="15"/>
-      <c r="B126" s="19"/>
+      <c r="B126" s="17"/>
       <c r="D126" s="8" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="15"/>
-      <c r="B127" s="19"/>
+      <c r="B127" s="17"/>
       <c r="D127" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="15"/>
-      <c r="B128" s="19"/>
+      <c r="B128" s="17"/>
       <c r="D128" s="8" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="15"/>
-      <c r="B129" s="19"/>
+      <c r="B129" s="17"/>
       <c r="D129" s="8"/>
     </row>
     <row r="130" spans="1:4">
@@ -3381,10 +3379,10 @@
       <c r="D141" s="8"/>
     </row>
     <row r="142" spans="1:4" ht="110" customHeight="1">
-      <c r="A142" s="22" t="s">
+      <c r="A142" t="s">
         <v>341</v>
       </c>
-      <c r="B142" s="22" t="s">
+      <c r="B142" t="s">
         <v>88</v>
       </c>
       <c r="D142" t="s">
@@ -3526,7 +3524,7 @@
       <c r="A162" s="14" t="s">
         <v>347</v>
       </c>
-      <c r="B162" s="18" t="s">
+      <c r="B162" s="16" t="s">
         <v>95</v>
       </c>
       <c r="D162" s="4" t="s">
@@ -3535,81 +3533,81 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="14"/>
-      <c r="B163" s="18"/>
+      <c r="B163" s="16"/>
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="14"/>
-      <c r="B164" s="18"/>
+      <c r="B164" s="16"/>
       <c r="D164" s="8" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="14"/>
-      <c r="B165" s="18"/>
+      <c r="B165" s="16"/>
       <c r="D165" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="14"/>
-      <c r="B166" s="18"/>
+      <c r="B166" s="16"/>
       <c r="D166" s="8" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="14"/>
-      <c r="B167" s="18"/>
+      <c r="B167" s="16"/>
       <c r="D167" s="8" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="14"/>
-      <c r="B168" s="18"/>
+      <c r="B168" s="16"/>
       <c r="D168" s="8" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="14"/>
-      <c r="B169" s="18"/>
+      <c r="B169" s="16"/>
       <c r="D169" s="8" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="14"/>
-      <c r="B170" s="18"/>
+      <c r="B170" s="16"/>
       <c r="D170" s="8" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="171" spans="1:4">
       <c r="A171" s="14"/>
-      <c r="B171" s="18"/>
+      <c r="B171" s="16"/>
       <c r="D171" s="8" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="172" spans="1:4">
       <c r="A172" s="14"/>
-      <c r="B172" s="18"/>
+      <c r="B172" s="16"/>
       <c r="D172" s="8" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="173" spans="1:4">
       <c r="A173" s="14"/>
-      <c r="B173" s="18"/>
+      <c r="B173" s="16"/>
       <c r="D173" s="8"/>
     </row>
     <row r="174" spans="1:4">
       <c r="A174" s="14" t="s">
         <v>348</v>
       </c>
-      <c r="B174" s="18" t="s">
+      <c r="B174" s="16" t="s">
         <v>103</v>
       </c>
       <c r="D174" s="4" t="s">
@@ -3618,39 +3616,39 @@
     </row>
     <row r="175" spans="1:4">
       <c r="A175" s="14"/>
-      <c r="B175" s="18"/>
+      <c r="B175" s="16"/>
     </row>
     <row r="176" spans="1:4">
       <c r="A176" s="14"/>
-      <c r="B176" s="18"/>
+      <c r="B176" s="16"/>
       <c r="D176" s="8" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="177" spans="1:4">
       <c r="A177" s="14"/>
-      <c r="B177" s="18"/>
+      <c r="B177" s="16"/>
       <c r="D177" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="178" spans="1:4">
       <c r="A178" s="14"/>
-      <c r="B178" s="18"/>
+      <c r="B178" s="16"/>
       <c r="D178" s="8" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="179" spans="1:4">
       <c r="A179" s="14"/>
-      <c r="B179" s="18"/>
+      <c r="B179" s="16"/>
       <c r="D179" s="8" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="180" spans="1:4">
       <c r="A180" s="14"/>
-      <c r="B180" s="18"/>
+      <c r="B180" s="16"/>
       <c r="D180" s="8"/>
     </row>
     <row r="181" spans="1:4">
@@ -3867,49 +3865,6 @@
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="A48:A92"/>
-    <mergeCell ref="B48:B92"/>
-    <mergeCell ref="A93:A104"/>
-    <mergeCell ref="B93:B104"/>
-    <mergeCell ref="A105:A129"/>
-    <mergeCell ref="B105:B129"/>
-    <mergeCell ref="A130:A133"/>
-    <mergeCell ref="B130:B133"/>
-    <mergeCell ref="A134:A137"/>
-    <mergeCell ref="B134:B137"/>
-    <mergeCell ref="A138:A141"/>
-    <mergeCell ref="B138:B141"/>
-    <mergeCell ref="A144:A148"/>
-    <mergeCell ref="B144:B148"/>
-    <mergeCell ref="B181:B184"/>
-    <mergeCell ref="A149:A153"/>
-    <mergeCell ref="B149:B153"/>
-    <mergeCell ref="A154:A157"/>
-    <mergeCell ref="B154:B157"/>
-    <mergeCell ref="A158:A161"/>
-    <mergeCell ref="B158:B161"/>
     <mergeCell ref="A201:A204"/>
     <mergeCell ref="B201:B204"/>
     <mergeCell ref="A205:A212"/>
@@ -3926,6 +3881,49 @@
     <mergeCell ref="A174:A180"/>
     <mergeCell ref="B174:B180"/>
     <mergeCell ref="A181:A184"/>
+    <mergeCell ref="B181:B184"/>
+    <mergeCell ref="A149:A153"/>
+    <mergeCell ref="B149:B153"/>
+    <mergeCell ref="A154:A157"/>
+    <mergeCell ref="B154:B157"/>
+    <mergeCell ref="A158:A161"/>
+    <mergeCell ref="B158:B161"/>
+    <mergeCell ref="A134:A137"/>
+    <mergeCell ref="B134:B137"/>
+    <mergeCell ref="A138:A141"/>
+    <mergeCell ref="B138:B141"/>
+    <mergeCell ref="A144:A148"/>
+    <mergeCell ref="B144:B148"/>
+    <mergeCell ref="A93:A104"/>
+    <mergeCell ref="B93:B104"/>
+    <mergeCell ref="A105:A129"/>
+    <mergeCell ref="B105:B129"/>
+    <mergeCell ref="A130:A133"/>
+    <mergeCell ref="B130:B133"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="A48:A92"/>
+    <mergeCell ref="B48:B92"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -3951,12 +3949,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1BA8D81-2B76-FE4E-BCA3-5D293CB987FF}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D60" sqref="D60"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4316,7 +4314,7 @@
         <v>159</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="4" t="s">
@@ -4493,42 +4491,6 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="B38:B40"/>
     <mergeCell ref="A51:A54"/>
     <mergeCell ref="B51:B54"/>
     <mergeCell ref="A41:A42"/>
@@ -4537,6 +4499,42 @@
     <mergeCell ref="B43:B44"/>
     <mergeCell ref="A45:A50"/>
     <mergeCell ref="B45:B50"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -4555,11 +4553,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEAF76D1-ED53-D146-BC1A-7722F4D40657}">
   <dimension ref="A1:C139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D34" sqref="D34"/>
+      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4585,7 +4583,7 @@
       <c r="A2" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="16" t="s">
         <v>299</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -4594,86 +4592,86 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="21"/>
-      <c r="B3" s="18"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="21"/>
-      <c r="B4" s="18"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="3" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="21"/>
-      <c r="B5" s="18"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="3" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="21"/>
-      <c r="B6" s="18"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="3" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="21"/>
-      <c r="B7" s="18"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="3" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="21"/>
-      <c r="B8" s="18"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="3">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="21"/>
-      <c r="B9" s="18"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="3" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="21"/>
-      <c r="B10" s="18"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="3" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="21"/>
-      <c r="B11" s="18"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="3" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="21"/>
-      <c r="B12" s="18"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="3" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="21"/>
-      <c r="B13" s="18"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="22" t="s">
         <v>300</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -4681,290 +4679,290 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="3" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="23"/>
-      <c r="B17" s="24"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="3" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="23"/>
-      <c r="B18" s="24"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="3" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="23"/>
-      <c r="B19" s="24"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="3" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="23"/>
-      <c r="B20" s="24"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="22"/>
       <c r="C20" s="3" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="23"/>
-      <c r="B21" s="24"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="22"/>
       <c r="C21" s="3" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="23"/>
-      <c r="B22" s="24"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="22"/>
       <c r="C22" s="3" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="23"/>
-      <c r="B23" s="24"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="22"/>
       <c r="C23" s="3" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="23"/>
-      <c r="B24" s="24"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="22"/>
       <c r="C24" s="3">
         <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="23"/>
-      <c r="B25" s="24"/>
+      <c r="A25" s="20"/>
+      <c r="B25" s="22"/>
       <c r="C25" s="3" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="23"/>
-      <c r="B26" s="24"/>
+      <c r="A26" s="20"/>
+      <c r="B26" s="22"/>
       <c r="C26" s="3" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="23"/>
-      <c r="B27" s="24"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="22"/>
       <c r="C27" s="3" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="23"/>
-      <c r="B28" s="24"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="22"/>
       <c r="C28" s="3" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="23"/>
-      <c r="B29" s="24"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="22"/>
       <c r="C29" s="3" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="23"/>
-      <c r="B30" s="24"/>
+      <c r="A30" s="20"/>
+      <c r="B30" s="22"/>
       <c r="C30" s="3" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="23"/>
-      <c r="B31" s="24"/>
+      <c r="A31" s="20"/>
+      <c r="B31" s="22"/>
       <c r="C31" s="3" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="23"/>
-      <c r="B32" s="24"/>
+      <c r="A32" s="20"/>
+      <c r="B32" s="22"/>
       <c r="C32" s="3" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="23"/>
-      <c r="B33" s="24"/>
+      <c r="A33" s="20"/>
+      <c r="B33" s="22"/>
       <c r="C33" s="3" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="23"/>
-      <c r="B34" s="24"/>
+      <c r="A34" s="20"/>
+      <c r="B34" s="22"/>
       <c r="C34" s="3" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="23"/>
-      <c r="B35" s="24"/>
+      <c r="A35" s="20"/>
+      <c r="B35" s="22"/>
       <c r="C35" s="3" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="23"/>
-      <c r="B36" s="24"/>
+      <c r="A36" s="20"/>
+      <c r="B36" s="22"/>
       <c r="C36" s="3" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="23"/>
-      <c r="B37" s="24"/>
+      <c r="A37" s="20"/>
+      <c r="B37" s="22"/>
       <c r="C37" s="3" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="23"/>
-      <c r="B38" s="24"/>
+      <c r="A38" s="20"/>
+      <c r="B38" s="22"/>
       <c r="C38" s="3" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="23"/>
-      <c r="B39" s="24"/>
+      <c r="A39" s="20"/>
+      <c r="B39" s="22"/>
       <c r="C39" s="3" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="23"/>
-      <c r="B40" s="24"/>
+      <c r="A40" s="20"/>
+      <c r="B40" s="22"/>
       <c r="C40" s="3" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="23"/>
-      <c r="B41" s="24"/>
+      <c r="A41" s="20"/>
+      <c r="B41" s="22"/>
       <c r="C41" s="3" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="23"/>
-      <c r="B42" s="24"/>
+      <c r="A42" s="20"/>
+      <c r="B42" s="22"/>
       <c r="C42" s="3" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="23"/>
-      <c r="B43" s="24"/>
+      <c r="A43" s="20"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="3" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="23"/>
-      <c r="B44" s="24"/>
+      <c r="A44" s="20"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="3" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="23"/>
-      <c r="B45" s="24"/>
+      <c r="A45" s="20"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="3" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="23"/>
-      <c r="B46" s="24"/>
+      <c r="A46" s="20"/>
+      <c r="B46" s="22"/>
       <c r="C46" s="3" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="23"/>
-      <c r="B47" s="24"/>
+      <c r="A47" s="20"/>
+      <c r="B47" s="22"/>
       <c r="C47" s="3" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="23"/>
-      <c r="B48" s="24"/>
+      <c r="A48" s="20"/>
+      <c r="B48" s="22"/>
       <c r="C48" s="3" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="23"/>
-      <c r="B49" s="24"/>
+      <c r="A49" s="20"/>
+      <c r="B49" s="22"/>
       <c r="C49" s="3" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="23"/>
-      <c r="B50" s="24"/>
+      <c r="A50" s="20"/>
+      <c r="B50" s="22"/>
       <c r="C50" s="3" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="23"/>
-      <c r="B51" s="24"/>
+      <c r="A51" s="20"/>
+      <c r="B51" s="22"/>
       <c r="C51" s="3" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="23"/>
-      <c r="B52" s="24"/>
+      <c r="A52" s="20"/>
+      <c r="B52" s="22"/>
       <c r="C52" s="3" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="23"/>
-      <c r="B53" s="24"/>
+      <c r="A53" s="20"/>
+      <c r="B53" s="22"/>
       <c r="C53" s="3" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="23"/>
-      <c r="B54" s="24"/>
+      <c r="A54" s="20"/>
+      <c r="B54" s="22"/>
       <c r="C54" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="18">
-      <c r="A55" s="23" t="s">
+      <c r="A55" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="B55" s="24" t="s">
+      <c r="B55" s="22" t="s">
         <v>301</v>
       </c>
       <c r="C55" s="2" t="s">
@@ -4972,249 +4970,249 @@
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="23"/>
-      <c r="B56" s="24"/>
+      <c r="A56" s="20"/>
+      <c r="B56" s="22"/>
     </row>
     <row r="57" spans="1:3" ht="18">
-      <c r="A57" s="23"/>
-      <c r="B57" s="24"/>
+      <c r="A57" s="20"/>
+      <c r="B57" s="22"/>
       <c r="C57" s="2" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="23"/>
-      <c r="B58" s="24"/>
+      <c r="A58" s="20"/>
+      <c r="B58" s="22"/>
       <c r="C58" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="23"/>
-      <c r="B59" s="24"/>
+      <c r="A59" s="20"/>
+      <c r="B59" s="22"/>
       <c r="C59" s="3" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="23"/>
-      <c r="B60" s="24"/>
+      <c r="A60" s="20"/>
+      <c r="B60" s="22"/>
       <c r="C60" s="3" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="23"/>
-      <c r="B61" s="24"/>
+      <c r="A61" s="20"/>
+      <c r="B61" s="22"/>
       <c r="C61" s="3" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="23"/>
-      <c r="B62" s="24"/>
+      <c r="A62" s="20"/>
+      <c r="B62" s="22"/>
       <c r="C62" s="3" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="23"/>
-      <c r="B63" s="24"/>
+      <c r="A63" s="20"/>
+      <c r="B63" s="22"/>
       <c r="C63" s="3">
         <v>52</v>
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="23"/>
-      <c r="B64" s="24"/>
+      <c r="A64" s="20"/>
+      <c r="B64" s="22"/>
       <c r="C64" s="3" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="23"/>
-      <c r="B65" s="24"/>
+      <c r="A65" s="20"/>
+      <c r="B65" s="22"/>
       <c r="C65" s="3" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="23"/>
-      <c r="B66" s="24"/>
+      <c r="A66" s="20"/>
+      <c r="B66" s="22"/>
       <c r="C66" s="3" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="23"/>
-      <c r="B67" s="24"/>
+      <c r="A67" s="20"/>
+      <c r="B67" s="22"/>
       <c r="C67" s="3" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="23"/>
-      <c r="B68" s="24"/>
+      <c r="A68" s="20"/>
+      <c r="B68" s="22"/>
       <c r="C68" s="3" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="23"/>
-      <c r="B69" s="24"/>
+      <c r="A69" s="20"/>
+      <c r="B69" s="22"/>
       <c r="C69" s="3" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="23"/>
-      <c r="B70" s="24"/>
+      <c r="A70" s="20"/>
+      <c r="B70" s="22"/>
       <c r="C70" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="23"/>
-      <c r="B71" s="24"/>
+      <c r="A71" s="20"/>
+      <c r="B71" s="22"/>
     </row>
     <row r="72" spans="1:3" ht="18">
-      <c r="A72" s="23"/>
-      <c r="B72" s="24"/>
+      <c r="A72" s="20"/>
+      <c r="B72" s="22"/>
       <c r="C72" s="2" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="23"/>
-      <c r="B73" s="24"/>
+      <c r="A73" s="20"/>
+      <c r="B73" s="22"/>
       <c r="C73" s="3" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="23"/>
-      <c r="B74" s="24"/>
+      <c r="A74" s="20"/>
+      <c r="B74" s="22"/>
       <c r="C74" s="3" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="23"/>
-      <c r="B75" s="24"/>
+      <c r="A75" s="20"/>
+      <c r="B75" s="22"/>
       <c r="C75" s="3" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="23"/>
-      <c r="B76" s="24"/>
+      <c r="A76" s="20"/>
+      <c r="B76" s="22"/>
       <c r="C76" s="3" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="23"/>
-      <c r="B77" s="24"/>
+      <c r="A77" s="20"/>
+      <c r="B77" s="22"/>
       <c r="C77" s="3" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="23"/>
-      <c r="B78" s="24"/>
+      <c r="A78" s="20"/>
+      <c r="B78" s="22"/>
       <c r="C78" s="3" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" s="23"/>
-      <c r="B79" s="24"/>
+      <c r="A79" s="20"/>
+      <c r="B79" s="22"/>
       <c r="C79" s="3" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" s="23"/>
-      <c r="B80" s="24"/>
+      <c r="A80" s="20"/>
+      <c r="B80" s="22"/>
       <c r="C80" s="3" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" s="23"/>
-      <c r="B81" s="24"/>
+      <c r="A81" s="20"/>
+      <c r="B81" s="22"/>
       <c r="C81" s="3" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="23"/>
-      <c r="B82" s="24"/>
+      <c r="A82" s="20"/>
+      <c r="B82" s="22"/>
       <c r="C82" s="3" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="23"/>
-      <c r="B83" s="24"/>
+      <c r="A83" s="20"/>
+      <c r="B83" s="22"/>
       <c r="C83" s="3" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" s="23"/>
-      <c r="B84" s="24"/>
+      <c r="A84" s="20"/>
+      <c r="B84" s="22"/>
       <c r="C84" s="3" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="23"/>
-      <c r="B85" s="24"/>
+      <c r="A85" s="20"/>
+      <c r="B85" s="22"/>
       <c r="C85" s="3" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="23"/>
-      <c r="B86" s="24"/>
+      <c r="A86" s="20"/>
+      <c r="B86" s="22"/>
       <c r="C86" s="3">
         <v>85</v>
       </c>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="23"/>
-      <c r="B87" s="24"/>
+      <c r="A87" s="20"/>
+      <c r="B87" s="22"/>
       <c r="C87" s="3" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" s="23"/>
-      <c r="B88" s="24"/>
+      <c r="A88" s="20"/>
+      <c r="B88" s="22"/>
       <c r="C88" s="3" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="23"/>
-      <c r="B89" s="24"/>
+      <c r="A89" s="20"/>
+      <c r="B89" s="22"/>
       <c r="C89" s="3" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" s="23"/>
-      <c r="B90" s="24"/>
+      <c r="A90" s="20"/>
+      <c r="B90" s="22"/>
       <c r="C90" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="18">
-      <c r="A91" s="23" t="s">
+      <c r="A91" s="20" t="s">
         <v>270</v>
       </c>
-      <c r="B91" s="24" t="s">
+      <c r="B91" s="22" t="s">
         <v>302</v>
       </c>
       <c r="C91" s="2" t="s">
@@ -5222,108 +5220,108 @@
       </c>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92" s="23"/>
-      <c r="B92" s="24"/>
+      <c r="A92" s="20"/>
+      <c r="B92" s="22"/>
       <c r="C92" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" s="23"/>
-      <c r="B93" s="24"/>
+      <c r="A93" s="20"/>
+      <c r="B93" s="22"/>
       <c r="C93" s="3" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" s="23"/>
-      <c r="B94" s="24"/>
+      <c r="A94" s="20"/>
+      <c r="B94" s="22"/>
       <c r="C94" s="3" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" s="23"/>
-      <c r="B95" s="24"/>
+      <c r="A95" s="20"/>
+      <c r="B95" s="22"/>
       <c r="C95" s="3" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" s="23"/>
-      <c r="B96" s="24"/>
+      <c r="A96" s="20"/>
+      <c r="B96" s="22"/>
       <c r="C96" s="3" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="23"/>
-      <c r="B97" s="24"/>
+      <c r="A97" s="20"/>
+      <c r="B97" s="22"/>
       <c r="C97" s="3" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" s="23"/>
-      <c r="B98" s="24"/>
+      <c r="A98" s="20"/>
+      <c r="B98" s="22"/>
       <c r="C98" s="3">
         <v>15</v>
       </c>
     </row>
     <row r="99" spans="1:3">
-      <c r="A99" s="23"/>
-      <c r="B99" s="24"/>
+      <c r="A99" s="20"/>
+      <c r="B99" s="22"/>
       <c r="C99" s="3" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="100" spans="1:3">
-      <c r="A100" s="23"/>
-      <c r="B100" s="24"/>
+      <c r="A100" s="20"/>
+      <c r="B100" s="22"/>
       <c r="C100" s="3" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="101" spans="1:3">
-      <c r="A101" s="23"/>
-      <c r="B101" s="24"/>
+      <c r="A101" s="20"/>
+      <c r="B101" s="22"/>
       <c r="C101" s="3" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="102" spans="1:3">
-      <c r="A102" s="23"/>
-      <c r="B102" s="24"/>
+      <c r="A102" s="20"/>
+      <c r="B102" s="22"/>
       <c r="C102" s="3" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="103" spans="1:3">
-      <c r="A103" s="23"/>
-      <c r="B103" s="24"/>
+      <c r="A103" s="20"/>
+      <c r="B103" s="22"/>
       <c r="C103" s="3" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="104" spans="1:3">
-      <c r="A104" s="23"/>
-      <c r="B104" s="24"/>
+      <c r="A104" s="20"/>
+      <c r="B104" s="22"/>
       <c r="C104" s="3" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="105" spans="1:3">
-      <c r="A105" s="23"/>
-      <c r="B105" s="24"/>
+      <c r="A105" s="20"/>
+      <c r="B105" s="22"/>
       <c r="C105" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="18">
-      <c r="A106" s="23" t="s">
+      <c r="A106" s="20" t="s">
         <v>278</v>
       </c>
-      <c r="B106" s="24" t="s">
+      <c r="B106" s="22" t="s">
         <v>303</v>
       </c>
       <c r="C106" s="2" t="s">
@@ -5331,87 +5329,87 @@
       </c>
     </row>
     <row r="107" spans="1:3">
-      <c r="A107" s="23"/>
-      <c r="B107" s="24"/>
+      <c r="A107" s="20"/>
+      <c r="B107" s="22"/>
       <c r="C107" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="108" spans="1:3">
-      <c r="A108" s="23"/>
-      <c r="B108" s="24"/>
+      <c r="A108" s="20"/>
+      <c r="B108" s="22"/>
       <c r="C108" s="3" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="109" spans="1:3">
-      <c r="A109" s="23"/>
-      <c r="B109" s="24"/>
+      <c r="A109" s="20"/>
+      <c r="B109" s="22"/>
       <c r="C109" s="3" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="110" spans="1:3">
-      <c r="A110" s="23"/>
-      <c r="B110" s="24"/>
+      <c r="A110" s="20"/>
+      <c r="B110" s="22"/>
       <c r="C110" s="3" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="111" spans="1:3">
-      <c r="A111" s="23"/>
-      <c r="B111" s="24"/>
+      <c r="A111" s="20"/>
+      <c r="B111" s="22"/>
       <c r="C111" s="3" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="112" spans="1:3">
-      <c r="A112" s="23"/>
-      <c r="B112" s="24"/>
+      <c r="A112" s="20"/>
+      <c r="B112" s="22"/>
       <c r="C112" s="3">
         <v>17</v>
       </c>
     </row>
     <row r="113" spans="1:3">
-      <c r="A113" s="23"/>
-      <c r="B113" s="24"/>
+      <c r="A113" s="20"/>
+      <c r="B113" s="22"/>
       <c r="C113" s="3" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="114" spans="1:3">
-      <c r="A114" s="23"/>
-      <c r="B114" s="24"/>
+      <c r="A114" s="20"/>
+      <c r="B114" s="22"/>
       <c r="C114" s="3" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="115" spans="1:3">
-      <c r="A115" s="23"/>
-      <c r="B115" s="24"/>
+      <c r="A115" s="20"/>
+      <c r="B115" s="22"/>
       <c r="C115" s="3" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="116" spans="1:3">
-      <c r="A116" s="23"/>
-      <c r="B116" s="24"/>
+      <c r="A116" s="20"/>
+      <c r="B116" s="22"/>
       <c r="C116" s="3" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="117" spans="1:3">
-      <c r="A117" s="23"/>
-      <c r="B117" s="24"/>
+      <c r="A117" s="20"/>
+      <c r="B117" s="22"/>
       <c r="C117" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="18">
-      <c r="A118" s="23" t="s">
+      <c r="A118" s="20" t="s">
         <v>283</v>
       </c>
-      <c r="B118" s="24" t="s">
+      <c r="B118" s="22" t="s">
         <v>304</v>
       </c>
       <c r="C118" s="2" t="s">
@@ -5419,166 +5417,166 @@
       </c>
     </row>
     <row r="119" spans="1:3">
-      <c r="A119" s="23"/>
-      <c r="B119" s="24"/>
+      <c r="A119" s="20"/>
+      <c r="B119" s="22"/>
       <c r="C119" s="3" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="120" spans="1:3">
-      <c r="A120" s="23"/>
-      <c r="B120" s="24"/>
+      <c r="A120" s="20"/>
+      <c r="B120" s="22"/>
       <c r="C120" s="3" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="121" spans="1:3">
-      <c r="A121" s="23"/>
-      <c r="B121" s="24"/>
+      <c r="A121" s="20"/>
+      <c r="B121" s="22"/>
       <c r="C121" s="3" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="122" spans="1:3">
-      <c r="A122" s="23"/>
-      <c r="B122" s="24"/>
+      <c r="A122" s="20"/>
+      <c r="B122" s="22"/>
       <c r="C122" s="3" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="123" spans="1:3">
-      <c r="A123" s="23"/>
-      <c r="B123" s="24"/>
+      <c r="A123" s="20"/>
+      <c r="B123" s="22"/>
       <c r="C123" s="3" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="124" spans="1:3">
-      <c r="A124" s="23"/>
-      <c r="B124" s="24"/>
+      <c r="A124" s="20"/>
+      <c r="B124" s="22"/>
       <c r="C124" s="3" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="125" spans="1:3">
-      <c r="A125" s="23"/>
-      <c r="B125" s="24"/>
+      <c r="A125" s="20"/>
+      <c r="B125" s="22"/>
       <c r="C125" s="3" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="126" spans="1:3">
-      <c r="A126" s="23"/>
-      <c r="B126" s="24"/>
+      <c r="A126" s="20"/>
+      <c r="B126" s="22"/>
       <c r="C126" s="3" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="127" spans="1:3">
-      <c r="A127" s="23"/>
-      <c r="B127" s="24"/>
+      <c r="A127" s="20"/>
+      <c r="B127" s="22"/>
       <c r="C127" s="3" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="128" spans="1:3">
-      <c r="A128" s="23"/>
-      <c r="B128" s="24"/>
+      <c r="A128" s="20"/>
+      <c r="B128" s="22"/>
       <c r="C128" s="3" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="129" spans="1:3">
-      <c r="A129" s="23"/>
-      <c r="B129" s="24"/>
+      <c r="A129" s="20"/>
+      <c r="B129" s="22"/>
       <c r="C129" s="3" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="130" spans="1:3">
-      <c r="A130" s="23"/>
-      <c r="B130" s="24"/>
+      <c r="A130" s="20"/>
+      <c r="B130" s="22"/>
       <c r="C130" s="3" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="131" spans="1:3">
-      <c r="A131" s="23"/>
-      <c r="B131" s="24"/>
+      <c r="A131" s="20"/>
+      <c r="B131" s="22"/>
       <c r="C131" s="3" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="132" spans="1:3">
-      <c r="A132" s="23"/>
-      <c r="B132" s="24"/>
+      <c r="A132" s="20"/>
+      <c r="B132" s="22"/>
       <c r="C132" s="3" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="133" spans="1:3">
-      <c r="A133" s="23"/>
-      <c r="B133" s="24"/>
+      <c r="A133" s="20"/>
+      <c r="B133" s="22"/>
       <c r="C133" s="3" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="134" spans="1:3">
-      <c r="A134" s="23"/>
-      <c r="B134" s="24"/>
+      <c r="A134" s="20"/>
+      <c r="B134" s="22"/>
       <c r="C134" s="3" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="135" spans="1:3">
-      <c r="A135" s="23"/>
-      <c r="B135" s="24"/>
+      <c r="A135" s="20"/>
+      <c r="B135" s="22"/>
       <c r="C135" s="3" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="136" spans="1:3">
-      <c r="A136" s="23"/>
-      <c r="B136" s="24"/>
+      <c r="A136" s="20"/>
+      <c r="B136" s="22"/>
       <c r="C136" s="3" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="137" spans="1:3">
-      <c r="A137" s="23"/>
-      <c r="B137" s="24"/>
+      <c r="A137" s="20"/>
+      <c r="B137" s="22"/>
       <c r="C137" s="3" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="138" spans="1:3">
-      <c r="A138" s="23"/>
-      <c r="B138" s="24"/>
+      <c r="A138" s="20"/>
+      <c r="B138" s="22"/>
       <c r="C138" s="3" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="139" spans="1:3">
-      <c r="A139" s="23"/>
-      <c r="B139" s="24"/>
+      <c r="A139" s="20"/>
+      <c r="B139" s="22"/>
       <c r="C139" s="3" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A91:A105"/>
+    <mergeCell ref="B91:B105"/>
+    <mergeCell ref="A106:A117"/>
+    <mergeCell ref="B106:B117"/>
+    <mergeCell ref="A118:A139"/>
+    <mergeCell ref="B118:B139"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A54"/>
     <mergeCell ref="B14:B54"/>
     <mergeCell ref="A55:A90"/>
     <mergeCell ref="B55:B90"/>
-    <mergeCell ref="A91:A105"/>
-    <mergeCell ref="B91:B105"/>
-    <mergeCell ref="A106:A117"/>
-    <mergeCell ref="B106:B117"/>
-    <mergeCell ref="A118:A139"/>
-    <mergeCell ref="B118:B139"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>